<commit_message>
Debugging multitracer data load test.  There are still issues, but the fixes thus far implkemented include:
Corrected the concentrations delimiter.
Split up isocorr tests from accucor.
Changed create_tracer_label to got_or_create_tracer_label.  Existing tracer label records were not being found because of the way the filtering was done in tracer.py.
Fixed the filter scheme in tracer.py.
  - It was combining all the filters with "and", which eliminated valid matches.

Files checked in: DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx DataRepo/models/tracer.py DataRepo/models/tracer_label.py DataRepo/tests/test_models.py DataRepo/utils/sample_table_loader.py
[skip ci]
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx
+++ b/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A454DF3-39AC-5548-8010-E63965A20121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2BB166F-030C-C040-9687-C63E29BDE329}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="44360" windowHeight="8940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="500" windowWidth="33200" windowHeight="15100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Treatments" sheetId="3" r:id="rId3"/>
     <sheet name="Tissues" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -40,7 +40,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Unique identifier for the animal (mouse) the sample was collected from. MUST match the Animal ID in the Animal Table.
 	-Lance Parsons</t>
@@ -54,7 +54,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The age of the animal (in weeks) at the time of sample collection
 	-Lance Parsons</t>
@@ -68,7 +68,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The sex of the animal ("male" or "female")
 	-Lance Parsons</t>
@@ -82,7 +82,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Genotype (optional)
 	-Lance Parsons</t>
@@ -96,7 +96,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Animal Body Weight (g) (optional)
 	-Lance Parsons</t>
@@ -110,7 +110,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The HMDB Common Name of the tracer compound infused into the animal
 	-Lance Parsons</t>
@@ -124,7 +124,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Concentration of infusate in this infusion solution (TODO: specify units)
 	-Lance Parsons
@@ -140,7 +140,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Volume of infusate solution infused in microliters (ul) per minute, per gram of mouse body weight
 	-Lance Parsons</t>
@@ -154,7 +154,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>The feeding descriptor for the animal [e.g. "LabDiet Rodent 5001"]
 	-Lance Parsons</t>
@@ -168,7 +168,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Animal feeding status: have the mice been fasted or fed?
 	-Lance Parsons
@@ -184,7 +184,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Short, unique identifier for an animal treatment protocol. Details should be provided in the Treatments table.
 	-Lance Parsons</t>
@@ -198,7 +198,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>An identifier for the "experiment", which is typically a collection of mice similar infusion parameters. this is loosely defined based on the person who did the infusions. Here, there is a consistant format: two initials for the lab member who did the infusion and then a number (date?)
 	-Lance Parsons</t>
@@ -212,7 +212,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>A long form description for the study which may include the experimental design process, citations, and other relevant details
 	-Lance Parsons</t>
@@ -236,7 +236,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Name of the sample, must match the sample name in AccuCor file
 	-Lance Parsons</t>
@@ -250,7 +250,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Date the sample was collected (YYYY-MM-DD)
 	-Lance Parsons</t>
@@ -264,7 +264,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Name of researcher who collected the sample
 	-Lance Parsons</t>
@@ -278,7 +278,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tissue type
 	-Lance Parsons
@@ -294,7 +294,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Minutes after infusion that the sample was collected
 	-Lance Parsons</t>
@@ -308,7 +308,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Unique identifier for the animal (mouse) the sample was collected from. MUST match the Animal ID in the Animal Table.
 	-Lance Parsons</t>
@@ -332,7 +332,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Short, unique identifier for an animal treatment protocol. Must match the values provided in the Animals table.
 	-Lance Parsons</t>
@@ -346,7 +346,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>A thorough description of an animal treatment protocol. This will be useful for searching and filtering, so use standard terms and be as complete as possible.
 	-Lance Parsons</t>
@@ -360,7 +360,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>this is an example treatment.  If this applies to your animal, please use this treatment.  If this does not apply to your animal, please add a new treatment.  Be as descriptive as possible.
 	-Michael Neinast</t>
@@ -384,7 +384,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>@mneinast@princeton.edu @matthewmcbride@princeton.edu - I believe I have seen datasets with both "BAT" and "iBAT", which I likely have erroneously merged. Should we add "bat_inquinal" or similar?
 _Assigned to Michael Neinast_
@@ -835,96 +835,6 @@
     <t>xz972-t</t>
   </si>
   <si>
-    <t>xz981-bat</t>
-  </si>
-  <si>
-    <t>xz981-br</t>
-  </si>
-  <si>
-    <t>xz981-dia</t>
-  </si>
-  <si>
-    <t>xz981-gas</t>
-  </si>
-  <si>
-    <t>xz981-gwat</t>
-  </si>
-  <si>
-    <t>xz981-h</t>
-  </si>
-  <si>
-    <t>xz981-kd</t>
-  </si>
-  <si>
-    <t>xz981-liv</t>
-  </si>
-  <si>
-    <t>xz981-lu</t>
-  </si>
-  <si>
-    <t>xz981-pc</t>
-  </si>
-  <si>
-    <t>xz981-q</t>
-  </si>
-  <si>
-    <t>xz981-si</t>
-  </si>
-  <si>
-    <t>xz981-sol</t>
-  </si>
-  <si>
-    <t>xz981-sp</t>
-  </si>
-  <si>
-    <t>xz981-t</t>
-  </si>
-  <si>
-    <t>xz982-bat</t>
-  </si>
-  <si>
-    <t>xz982-br</t>
-  </si>
-  <si>
-    <t>xz982-dia</t>
-  </si>
-  <si>
-    <t>xz982-gas</t>
-  </si>
-  <si>
-    <t>xz982-gwat</t>
-  </si>
-  <si>
-    <t>xz982-h</t>
-  </si>
-  <si>
-    <t>xz982-kd</t>
-  </si>
-  <si>
-    <t>xz982-liv</t>
-  </si>
-  <si>
-    <t>xz982-lu</t>
-  </si>
-  <si>
-    <t>xz982-pc</t>
-  </si>
-  <si>
-    <t>xz982-q</t>
-  </si>
-  <si>
-    <t>xz982-si</t>
-  </si>
-  <si>
-    <t>xz982-sol</t>
-  </si>
-  <si>
-    <t>xz982-sp</t>
-  </si>
-  <si>
-    <t>xz982-t</t>
-  </si>
-  <si>
     <t>Treatment Description</t>
   </si>
   <si>
@@ -1070,6 +980,96 @@
   </si>
   <si>
     <t>14; 18; 5; 23; 10; 15</t>
+  </si>
+  <si>
+    <t>xz981_bat</t>
+  </si>
+  <si>
+    <t>xz981_br</t>
+  </si>
+  <si>
+    <t>xz981_dia</t>
+  </si>
+  <si>
+    <t>xz981_gas</t>
+  </si>
+  <si>
+    <t>xz981_gwat</t>
+  </si>
+  <si>
+    <t>xz981_h</t>
+  </si>
+  <si>
+    <t>xz981_kd</t>
+  </si>
+  <si>
+    <t>xz981_liv</t>
+  </si>
+  <si>
+    <t>xz981_lu</t>
+  </si>
+  <si>
+    <t>xz981_pc</t>
+  </si>
+  <si>
+    <t>xz981_q</t>
+  </si>
+  <si>
+    <t>xz981_si</t>
+  </si>
+  <si>
+    <t>xz981_sol</t>
+  </si>
+  <si>
+    <t>xz981_sp</t>
+  </si>
+  <si>
+    <t>xz981_t</t>
+  </si>
+  <si>
+    <t>xz982_bat</t>
+  </si>
+  <si>
+    <t>xz982_br</t>
+  </si>
+  <si>
+    <t>xz982_dia</t>
+  </si>
+  <si>
+    <t>xz982_gas</t>
+  </si>
+  <si>
+    <t>xz982_gwat</t>
+  </si>
+  <si>
+    <t>xz982_h</t>
+  </si>
+  <si>
+    <t>xz982_kd</t>
+  </si>
+  <si>
+    <t>xz982_liv</t>
+  </si>
+  <si>
+    <t>xz982_lu</t>
+  </si>
+  <si>
+    <t>xz982_pc</t>
+  </si>
+  <si>
+    <t>xz982_q</t>
+  </si>
+  <si>
+    <t>xz982_si</t>
+  </si>
+  <si>
+    <t>xz982_sol</t>
+  </si>
+  <si>
+    <t>xz982_sp</t>
+  </si>
+  <si>
+    <t>xz982_t</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1079,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1091,38 +1091,44 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF9900"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF34A853"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1551,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ955"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
@@ -1634,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="H2">
         <v>0.115</v>
@@ -1675,7 +1681,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="H3">
         <v>0.109</v>
@@ -1716,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="H4">
         <v>6.0999999999999999E-2</v>
@@ -1757,7 +1763,7 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="H5">
         <v>5.8000000000000003E-2</v>
@@ -1798,7 +1804,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="H6">
         <v>0.114</v>
@@ -1839,7 +1845,7 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="H7">
         <v>0.11700000000000001</v>
@@ -1880,7 +1886,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="H8">
         <v>6.0999999999999999E-2</v>
@@ -1921,7 +1927,7 @@
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="H9">
         <v>0.06</v>
@@ -5747,9 +5753,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD400"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8926,7 +8932,7 @@
     </row>
     <row r="92" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="9" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="B92" s="10">
         <v>44169</v>
@@ -8970,7 +8976,7 @@
     </row>
     <row r="93" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="9" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="B93" s="10">
         <v>44169</v>
@@ -9014,7 +9020,7 @@
     </row>
     <row r="94" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="9" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="B94" s="10">
         <v>44169</v>
@@ -9058,7 +9064,7 @@
     </row>
     <row r="95" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="9" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="B95" s="10">
         <v>44169</v>
@@ -9102,7 +9108,7 @@
     </row>
     <row r="96" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A96" s="9" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="B96" s="10">
         <v>44169</v>
@@ -9146,7 +9152,7 @@
     </row>
     <row r="97" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="9" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="B97" s="10">
         <v>44169</v>
@@ -9190,7 +9196,7 @@
     </row>
     <row r="98" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="9" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="B98" s="10">
         <v>44169</v>
@@ -9234,7 +9240,7 @@
     </row>
     <row r="99" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A99" s="9" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="B99" s="10">
         <v>44169</v>
@@ -9278,7 +9284,7 @@
     </row>
     <row r="100" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="9" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
       <c r="B100" s="10">
         <v>44169</v>
@@ -9322,7 +9328,7 @@
     </row>
     <row r="101" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="9" t="s">
-        <v>153</v>
+        <v>202</v>
       </c>
       <c r="B101" s="10">
         <v>44169</v>
@@ -9366,7 +9372,7 @@
     </row>
     <row r="102" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="9" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="B102" s="10">
         <v>44169</v>
@@ -9410,7 +9416,7 @@
     </row>
     <row r="103" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="9" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="B103" s="10">
         <v>44169</v>
@@ -9454,7 +9460,7 @@
     </row>
     <row r="104" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="9" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="B104" s="10">
         <v>44169</v>
@@ -9498,7 +9504,7 @@
     </row>
     <row r="105" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="9" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="B105" s="10">
         <v>44169</v>
@@ -9542,7 +9548,7 @@
     </row>
     <row r="106" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="9" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="B106" s="10">
         <v>44169</v>
@@ -9586,7 +9592,7 @@
     </row>
     <row r="107" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="9" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="B107" s="10">
         <v>44169</v>
@@ -9630,7 +9636,7 @@
     </row>
     <row r="108" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="9" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="B108" s="10">
         <v>44169</v>
@@ -9674,7 +9680,7 @@
     </row>
     <row r="109" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="9" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="B109" s="10">
         <v>44169</v>
@@ -9718,7 +9724,7 @@
     </row>
     <row r="110" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A110" s="9" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="B110" s="10">
         <v>44169</v>
@@ -9762,7 +9768,7 @@
     </row>
     <row r="111" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="9" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="B111" s="10">
         <v>44169</v>
@@ -9806,7 +9812,7 @@
     </row>
     <row r="112" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A112" s="9" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="B112" s="10">
         <v>44169</v>
@@ -9850,7 +9856,7 @@
     </row>
     <row r="113" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="9" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="B113" s="10">
         <v>44169</v>
@@ -9894,7 +9900,7 @@
     </row>
     <row r="114" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A114" s="9" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="B114" s="10">
         <v>44169</v>
@@ -9938,7 +9944,7 @@
     </row>
     <row r="115" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="9" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="B115" s="10">
         <v>44169</v>
@@ -9982,7 +9988,7 @@
     </row>
     <row r="116" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="9" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="B116" s="10">
         <v>44169</v>
@@ -10026,7 +10032,7 @@
     </row>
     <row r="117" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="9" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="B117" s="10">
         <v>44169</v>
@@ -10070,7 +10076,7 @@
     </row>
     <row r="118" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A118" s="9" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="B118" s="10">
         <v>44169</v>
@@ -10114,7 +10120,7 @@
     </row>
     <row r="119" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="9" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="B119" s="10">
         <v>44169</v>
@@ -10158,7 +10164,7 @@
     </row>
     <row r="120" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A120" s="9" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="B120" s="10">
         <v>44169</v>
@@ -10202,7 +10208,7 @@
     </row>
     <row r="121" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A121" s="9" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="B121" s="10">
         <v>44169</v>
@@ -15327,7 +15333,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -15359,7 +15365,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -15387,10 +15393,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="5"/>
@@ -15421,7 +15427,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="D2" s="15"/>
     </row>
@@ -15430,7 +15436,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="D3" s="15"/>
     </row>
@@ -15439,7 +15445,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D4" s="15"/>
     </row>
@@ -15448,7 +15454,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="D5" s="15"/>
     </row>
@@ -15457,7 +15463,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="D6" s="15"/>
     </row>
@@ -15466,7 +15472,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="D7" s="15"/>
     </row>
@@ -15511,7 +15517,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="D12" s="15"/>
     </row>
@@ -15520,7 +15526,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D13" s="15"/>
     </row>
@@ -15535,34 +15541,34 @@
     </row>
     <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14" x14ac:dyDescent="0.15">
@@ -15578,135 +15584,135 @@
         <v>68</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remaining tests for multitracer and multilabel data.
Files checked in: DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx DataRepo/tests/test_infusate_parsing_validation.py DataRepo/tests/test_models.py DataRepo/utils/accucor_data_loader.py
[skip ci]
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx
+++ b/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/animal_sample_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/obob_fasted_ace_glycerol_3hb_citrate_eaa_fa_multiple_tracers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2BB166F-030C-C040-9687-C63E29BDE329}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDD34FA-8378-EF43-BF0E-80DD814FD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="500" windowWidth="33200" windowHeight="15100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="500" windowWidth="33200" windowHeight="26920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Treatments" sheetId="3" r:id="rId3"/>
     <sheet name="Tissues" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -514,9 +514,6 @@
     <t>Collection Time</t>
   </si>
   <si>
-    <t>xz1078-bat</t>
-  </si>
-  <si>
     <t>Xianfeng Zeng</t>
   </si>
   <si>
@@ -526,315 +523,48 @@
     <t>150</t>
   </si>
   <si>
-    <t>xz1078-br</t>
-  </si>
-  <si>
     <t>brain</t>
   </si>
   <si>
-    <t>xz1078-dia</t>
-  </si>
-  <si>
     <t>diaphragm</t>
   </si>
   <si>
-    <t>xz1078-gas</t>
-  </si>
-  <si>
     <t>gastrocnemius</t>
   </si>
   <si>
-    <t>xz1078-gwat</t>
-  </si>
-  <si>
     <t>white_adipose_tissue_gonadal</t>
   </si>
   <si>
-    <t>xz1078-h</t>
-  </si>
-  <si>
     <t>heart</t>
   </si>
   <si>
-    <t>xz1078-kd</t>
-  </si>
-  <si>
     <t>kidney</t>
   </si>
   <si>
-    <t>xz1078-liv</t>
-  </si>
-  <si>
     <t>liver</t>
   </si>
   <si>
-    <t>xz1078-lu</t>
-  </si>
-  <si>
     <t>lung</t>
   </si>
   <si>
-    <t>xz1078-pc</t>
-  </si>
-  <si>
     <t>pancreas</t>
   </si>
   <si>
-    <t>xz1078-q</t>
-  </si>
-  <si>
     <t>quadricep</t>
   </si>
   <si>
-    <t>xz1078-si</t>
-  </si>
-  <si>
     <t>small_intestine</t>
   </si>
   <si>
-    <t>xz1078-sol</t>
-  </si>
-  <si>
     <t>soleus</t>
   </si>
   <si>
-    <t>xz1078-sp</t>
-  </si>
-  <si>
     <t>spleen</t>
   </si>
   <si>
-    <t>xz1078-t</t>
-  </si>
-  <si>
     <t>serum_plasma_tail</t>
   </si>
   <si>
-    <t>xz1079-bat</t>
-  </si>
-  <si>
-    <t>xz1079-br</t>
-  </si>
-  <si>
-    <t>xz1079-dia</t>
-  </si>
-  <si>
-    <t>xz1079-gas</t>
-  </si>
-  <si>
-    <t>xz1079-gwat</t>
-  </si>
-  <si>
-    <t>xz1079-h</t>
-  </si>
-  <si>
-    <t>xz1079-kd</t>
-  </si>
-  <si>
-    <t>xz1079-liv</t>
-  </si>
-  <si>
-    <t>xz1079-lu</t>
-  </si>
-  <si>
-    <t>xz1079-pc</t>
-  </si>
-  <si>
-    <t>xz1079-q</t>
-  </si>
-  <si>
-    <t>xz1079-si</t>
-  </si>
-  <si>
-    <t>xz1079-sol</t>
-  </si>
-  <si>
-    <t>xz1079-sp</t>
-  </si>
-  <si>
-    <t>xz1079-t</t>
-  </si>
-  <si>
-    <t>xz1080-bat</t>
-  </si>
-  <si>
-    <t>xz1080-br</t>
-  </si>
-  <si>
-    <t>xz1080-dia</t>
-  </si>
-  <si>
-    <t>xz1080-gas</t>
-  </si>
-  <si>
-    <t>xz1080-gwat</t>
-  </si>
-  <si>
-    <t>xz1080-h</t>
-  </si>
-  <si>
-    <t>xz1080-kd</t>
-  </si>
-  <si>
-    <t>xz1080-liv</t>
-  </si>
-  <si>
-    <t>xz1080-lu</t>
-  </si>
-  <si>
-    <t>xz1080-pc</t>
-  </si>
-  <si>
-    <t>xz1080-q</t>
-  </si>
-  <si>
-    <t>xz1080-si</t>
-  </si>
-  <si>
-    <t>xz1080-sol</t>
-  </si>
-  <si>
-    <t>xz1080-sp</t>
-  </si>
-  <si>
-    <t>xz1080-t</t>
-  </si>
-  <si>
-    <t>xz1081-bat</t>
-  </si>
-  <si>
-    <t>xz1081-br</t>
-  </si>
-  <si>
-    <t>xz1081-dia</t>
-  </si>
-  <si>
-    <t>xz1081-gas</t>
-  </si>
-  <si>
-    <t>xz1081-gwat</t>
-  </si>
-  <si>
-    <t>xz1081-h</t>
-  </si>
-  <si>
-    <t>xz1081-kd</t>
-  </si>
-  <si>
-    <t>xz1081-liv</t>
-  </si>
-  <si>
-    <t>xz1081-lu</t>
-  </si>
-  <si>
-    <t>xz1081-pc</t>
-  </si>
-  <si>
-    <t>xz1081-q</t>
-  </si>
-  <si>
-    <t>xz1081-si</t>
-  </si>
-  <si>
-    <t>xz1081-sol</t>
-  </si>
-  <si>
-    <t>xz1081-sp</t>
-  </si>
-  <si>
-    <t>xz1081-t</t>
-  </si>
-  <si>
-    <t>xz971-bat</t>
-  </si>
-  <si>
-    <t>xz971-br</t>
-  </si>
-  <si>
-    <t>xz971-dia</t>
-  </si>
-  <si>
-    <t>xz971-gas</t>
-  </si>
-  <si>
-    <t>xz971-gwat</t>
-  </si>
-  <si>
-    <t>xz971-h</t>
-  </si>
-  <si>
-    <t>xz971-kd</t>
-  </si>
-  <si>
-    <t>xz971-liv</t>
-  </si>
-  <si>
-    <t>xz971-lu</t>
-  </si>
-  <si>
-    <t>xz971-pc</t>
-  </si>
-  <si>
-    <t>xz971-q</t>
-  </si>
-  <si>
-    <t>xz971-si</t>
-  </si>
-  <si>
-    <t>xz971-sol</t>
-  </si>
-  <si>
-    <t>xz971-sp</t>
-  </si>
-  <si>
-    <t>xz971-t</t>
-  </si>
-  <si>
-    <t>xz972-bat</t>
-  </si>
-  <si>
-    <t>xz972-br</t>
-  </si>
-  <si>
-    <t>xz972-dia</t>
-  </si>
-  <si>
-    <t>xz972-gas</t>
-  </si>
-  <si>
-    <t>xz972-gwat</t>
-  </si>
-  <si>
-    <t>xz972-h</t>
-  </si>
-  <si>
-    <t>xz972-kd</t>
-  </si>
-  <si>
-    <t>xz972-liv</t>
-  </si>
-  <si>
-    <t>xz972-lu</t>
-  </si>
-  <si>
-    <t>xz972-pc</t>
-  </si>
-  <si>
-    <t>xz972-q</t>
-  </si>
-  <si>
-    <t>xz972-si</t>
-  </si>
-  <si>
-    <t>xz972-sol</t>
-  </si>
-  <si>
-    <t>xz972-sp</t>
-  </si>
-  <si>
-    <t>xz972-t</t>
-  </si>
-  <si>
     <t>Treatment Description</t>
   </si>
   <si>
@@ -1070,6 +800,276 @@
   </si>
   <si>
     <t>xz982_t</t>
+  </si>
+  <si>
+    <t>xz971_bat</t>
+  </si>
+  <si>
+    <t>xz971_br</t>
+  </si>
+  <si>
+    <t>xz971_dia</t>
+  </si>
+  <si>
+    <t>xz971_gas</t>
+  </si>
+  <si>
+    <t>xz971_gwat</t>
+  </si>
+  <si>
+    <t>xz971_h</t>
+  </si>
+  <si>
+    <t>xz971_kd</t>
+  </si>
+  <si>
+    <t>xz971_liv</t>
+  </si>
+  <si>
+    <t>xz971_lu</t>
+  </si>
+  <si>
+    <t>xz971_pc</t>
+  </si>
+  <si>
+    <t>xz971_q</t>
+  </si>
+  <si>
+    <t>xz971_si</t>
+  </si>
+  <si>
+    <t>xz971_sol</t>
+  </si>
+  <si>
+    <t>xz971_sp</t>
+  </si>
+  <si>
+    <t>xz971_t</t>
+  </si>
+  <si>
+    <t>xz972_bat</t>
+  </si>
+  <si>
+    <t>xz972_br</t>
+  </si>
+  <si>
+    <t>xz972_dia</t>
+  </si>
+  <si>
+    <t>xz972_gas</t>
+  </si>
+  <si>
+    <t>xz972_gwat</t>
+  </si>
+  <si>
+    <t>xz972_h</t>
+  </si>
+  <si>
+    <t>xz972_kd</t>
+  </si>
+  <si>
+    <t>xz972_liv</t>
+  </si>
+  <si>
+    <t>xz972_lu</t>
+  </si>
+  <si>
+    <t>xz972_pc</t>
+  </si>
+  <si>
+    <t>xz972_q</t>
+  </si>
+  <si>
+    <t>xz972_si</t>
+  </si>
+  <si>
+    <t>xz972_sol</t>
+  </si>
+  <si>
+    <t>xz972_sp</t>
+  </si>
+  <si>
+    <t>xz972_t</t>
+  </si>
+  <si>
+    <t>xz1078_bat</t>
+  </si>
+  <si>
+    <t>xz1078_br</t>
+  </si>
+  <si>
+    <t>xz1078_dia</t>
+  </si>
+  <si>
+    <t>xz1078_gas</t>
+  </si>
+  <si>
+    <t>xz1078_gwat</t>
+  </si>
+  <si>
+    <t>xz1078_h</t>
+  </si>
+  <si>
+    <t>xz1078_kd</t>
+  </si>
+  <si>
+    <t>xz1078_liv</t>
+  </si>
+  <si>
+    <t>xz1078_lu</t>
+  </si>
+  <si>
+    <t>xz1078_pc</t>
+  </si>
+  <si>
+    <t>xz1078_q</t>
+  </si>
+  <si>
+    <t>xz1078_si</t>
+  </si>
+  <si>
+    <t>xz1078_sol</t>
+  </si>
+  <si>
+    <t>xz1078_sp</t>
+  </si>
+  <si>
+    <t>xz1078_t</t>
+  </si>
+  <si>
+    <t>xz1079_bat</t>
+  </si>
+  <si>
+    <t>xz1079_br</t>
+  </si>
+  <si>
+    <t>xz1079_dia</t>
+  </si>
+  <si>
+    <t>xz1079_gas</t>
+  </si>
+  <si>
+    <t>xz1079_gwat</t>
+  </si>
+  <si>
+    <t>xz1079_h</t>
+  </si>
+  <si>
+    <t>xz1079_kd</t>
+  </si>
+  <si>
+    <t>xz1079_liv</t>
+  </si>
+  <si>
+    <t>xz1079_lu</t>
+  </si>
+  <si>
+    <t>xz1079_pc</t>
+  </si>
+  <si>
+    <t>xz1079_q</t>
+  </si>
+  <si>
+    <t>xz1079_si</t>
+  </si>
+  <si>
+    <t>xz1079_sol</t>
+  </si>
+  <si>
+    <t>xz1079_sp</t>
+  </si>
+  <si>
+    <t>xz1079_t</t>
+  </si>
+  <si>
+    <t>xz1080_bat</t>
+  </si>
+  <si>
+    <t>xz1080_br</t>
+  </si>
+  <si>
+    <t>xz1080_dia</t>
+  </si>
+  <si>
+    <t>xz1080_gas</t>
+  </si>
+  <si>
+    <t>xz1080_gwat</t>
+  </si>
+  <si>
+    <t>xz1080_h</t>
+  </si>
+  <si>
+    <t>xz1080_kd</t>
+  </si>
+  <si>
+    <t>xz1080_liv</t>
+  </si>
+  <si>
+    <t>xz1080_lu</t>
+  </si>
+  <si>
+    <t>xz1080_pc</t>
+  </si>
+  <si>
+    <t>xz1080_q</t>
+  </si>
+  <si>
+    <t>xz1080_si</t>
+  </si>
+  <si>
+    <t>xz1080_sol</t>
+  </si>
+  <si>
+    <t>xz1080_sp</t>
+  </si>
+  <si>
+    <t>xz1080_t</t>
+  </si>
+  <si>
+    <t>xz1081_bat</t>
+  </si>
+  <si>
+    <t>xz1081_br</t>
+  </si>
+  <si>
+    <t>xz1081_dia</t>
+  </si>
+  <si>
+    <t>xz1081_gas</t>
+  </si>
+  <si>
+    <t>xz1081_gwat</t>
+  </si>
+  <si>
+    <t>xz1081_h</t>
+  </si>
+  <si>
+    <t>xz1081_kd</t>
+  </si>
+  <si>
+    <t>xz1081_liv</t>
+  </si>
+  <si>
+    <t>xz1081_lu</t>
+  </si>
+  <si>
+    <t>xz1081_pc</t>
+  </si>
+  <si>
+    <t>xz1081_q</t>
+  </si>
+  <si>
+    <t>xz1081_si</t>
+  </si>
+  <si>
+    <t>xz1081_sol</t>
+  </si>
+  <si>
+    <t>xz1081_sp</t>
+  </si>
+  <si>
+    <t>xz1081_t</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="H2">
         <v>0.115</v>
@@ -1681,7 +1681,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="H3">
         <v>0.109</v>
@@ -1722,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="H4">
         <v>6.0999999999999999E-2</v>
@@ -1763,7 +1763,7 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="H5">
         <v>5.8000000000000003E-2</v>
@@ -1804,7 +1804,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="H6">
         <v>0.114</v>
@@ -1845,7 +1845,7 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="H7">
         <v>0.11700000000000001</v>
@@ -1886,7 +1886,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="H8">
         <v>6.0999999999999999E-2</v>
@@ -1927,7 +1927,7 @@
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="H9">
         <v>0.06</v>
@@ -5754,8 +5754,8 @@
   <dimension ref="A1:AD400"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5812,19 +5812,19 @@
     </row>
     <row r="2" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7">
         <v>44316</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>23</v>
@@ -5842,19 +5842,19 @@
     </row>
     <row r="3" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="B3" s="7">
         <v>44316</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>23</v>
@@ -5872,19 +5872,19 @@
     </row>
     <row r="4" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="B4" s="7">
         <v>44316</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>23</v>
@@ -5902,19 +5902,19 @@
     </row>
     <row r="5" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="B5" s="7">
         <v>44316</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>23</v>
@@ -5932,19 +5932,19 @@
     </row>
     <row r="6" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="B6" s="7">
         <v>44316</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>23</v>
@@ -5962,19 +5962,19 @@
     </row>
     <row r="7" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>49</v>
+        <v>168</v>
       </c>
       <c r="B7" s="7">
         <v>44316</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>23</v>
@@ -5992,19 +5992,19 @@
     </row>
     <row r="8" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>51</v>
+        <v>169</v>
       </c>
       <c r="B8" s="7">
         <v>44316</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>23</v>
@@ -6022,19 +6022,19 @@
     </row>
     <row r="9" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="B9" s="7">
         <v>44316</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>23</v>
@@ -6052,19 +6052,19 @@
     </row>
     <row r="10" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
-        <v>55</v>
+        <v>171</v>
       </c>
       <c r="B10" s="7">
         <v>44316</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>23</v>
@@ -6082,19 +6082,19 @@
     </row>
     <row r="11" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="B11" s="7">
         <v>44316</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>23</v>
@@ -6112,19 +6112,19 @@
     </row>
     <row r="12" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="B12" s="7">
         <v>44316</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>23</v>
@@ -6142,19 +6142,19 @@
     </row>
     <row r="13" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="B13" s="7">
         <v>44316</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>23</v>
@@ -6172,19 +6172,19 @@
     </row>
     <row r="14" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>63</v>
+        <v>175</v>
       </c>
       <c r="B14" s="7">
         <v>44316</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>23</v>
@@ -6202,19 +6202,19 @@
     </row>
     <row r="15" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="B15" s="7">
         <v>44316</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>23</v>
@@ -6232,19 +6232,19 @@
     </row>
     <row r="16" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="B16" s="7">
         <v>44316</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>23</v>
@@ -6262,19 +6262,19 @@
     </row>
     <row r="17" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="B17" s="7">
         <v>44316</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>13</v>
@@ -6292,19 +6292,19 @@
     </row>
     <row r="18" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>70</v>
+        <v>179</v>
       </c>
       <c r="B18" s="7">
         <v>44316</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>13</v>
@@ -6322,19 +6322,19 @@
     </row>
     <row r="19" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>180</v>
       </c>
       <c r="B19" s="7">
         <v>44316</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>13</v>
@@ -6352,19 +6352,19 @@
     </row>
     <row r="20" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="B20" s="7">
         <v>44316</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>13</v>
@@ -6382,19 +6382,19 @@
     </row>
     <row r="21" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="B21" s="7">
         <v>44316</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>13</v>
@@ -6412,19 +6412,19 @@
     </row>
     <row r="22" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>74</v>
+        <v>183</v>
       </c>
       <c r="B22" s="7">
         <v>44316</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>13</v>
@@ -6442,19 +6442,19 @@
     </row>
     <row r="23" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="B23" s="7">
         <v>44316</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>13</v>
@@ -6472,19 +6472,19 @@
     </row>
     <row r="24" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>76</v>
+        <v>185</v>
       </c>
       <c r="B24" s="7">
         <v>44316</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>13</v>
@@ -6502,19 +6502,19 @@
     </row>
     <row r="25" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="B25" s="7">
         <v>44316</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>13</v>
@@ -6532,19 +6532,19 @@
     </row>
     <row r="26" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>78</v>
+        <v>187</v>
       </c>
       <c r="B26" s="7">
         <v>44316</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>13</v>
@@ -6562,19 +6562,19 @@
     </row>
     <row r="27" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="B27" s="7">
         <v>44316</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>13</v>
@@ -6592,19 +6592,19 @@
     </row>
     <row r="28" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="B28" s="7">
         <v>44316</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>13</v>
@@ -6622,19 +6622,19 @@
     </row>
     <row r="29" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="B29" s="7">
         <v>44316</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>13</v>
@@ -6652,19 +6652,19 @@
     </row>
     <row r="30" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>82</v>
+        <v>191</v>
       </c>
       <c r="B30" s="7">
         <v>44316</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>13</v>
@@ -6682,19 +6682,19 @@
     </row>
     <row r="31" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="B31" s="7">
         <v>44316</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>13</v>
@@ -6712,19 +6712,19 @@
     </row>
     <row r="32" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="B32" s="7">
         <v>44316</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>22</v>
@@ -6742,19 +6742,19 @@
     </row>
     <row r="33" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="B33" s="7">
         <v>44316</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>22</v>
@@ -6772,19 +6772,19 @@
     </row>
     <row r="34" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>86</v>
+        <v>195</v>
       </c>
       <c r="B34" s="7">
         <v>44316</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>22</v>
@@ -6802,19 +6802,19 @@
     </row>
     <row r="35" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="B35" s="7">
         <v>44316</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
@@ -6832,19 +6832,19 @@
     </row>
     <row r="36" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="B36" s="7">
         <v>44316</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>22</v>
@@ -6862,19 +6862,19 @@
     </row>
     <row r="37" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="B37" s="7">
         <v>44316</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>22</v>
@@ -6892,19 +6892,19 @@
     </row>
     <row r="38" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>90</v>
+        <v>199</v>
       </c>
       <c r="B38" s="7">
         <v>44316</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>22</v>
@@ -6922,19 +6922,19 @@
     </row>
     <row r="39" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="B39" s="7">
         <v>44316</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>22</v>
@@ -6952,19 +6952,19 @@
     </row>
     <row r="40" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>92</v>
+        <v>201</v>
       </c>
       <c r="B40" s="7">
         <v>44316</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>22</v>
@@ -6982,19 +6982,19 @@
     </row>
     <row r="41" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
       <c r="B41" s="7">
         <v>44316</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>22</v>
@@ -7012,19 +7012,19 @@
     </row>
     <row r="42" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>94</v>
+        <v>203</v>
       </c>
       <c r="B42" s="7">
         <v>44316</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>22</v>
@@ -7042,19 +7042,19 @@
     </row>
     <row r="43" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="B43" s="7">
         <v>44316</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>22</v>
@@ -7072,19 +7072,19 @@
     </row>
     <row r="44" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>96</v>
+        <v>205</v>
       </c>
       <c r="B44" s="7">
         <v>44316</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>22</v>
@@ -7102,19 +7102,19 @@
     </row>
     <row r="45" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>97</v>
+        <v>206</v>
       </c>
       <c r="B45" s="7">
         <v>44316</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>22</v>
@@ -7132,19 +7132,19 @@
     </row>
     <row r="46" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="B46" s="7">
         <v>44316</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>22</v>
@@ -7162,19 +7162,19 @@
     </row>
     <row r="47" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>99</v>
+        <v>208</v>
       </c>
       <c r="B47" s="7">
         <v>44316</v>
       </c>
       <c r="C47" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>25</v>
@@ -7192,19 +7192,19 @@
     </row>
     <row r="48" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>100</v>
+        <v>209</v>
       </c>
       <c r="B48" s="7">
         <v>44316</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>25</v>
@@ -7222,19 +7222,19 @@
     </row>
     <row r="49" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>101</v>
+        <v>210</v>
       </c>
       <c r="B49" s="7">
         <v>44316</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>25</v>
@@ -7252,19 +7252,19 @@
     </row>
     <row r="50" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>102</v>
+        <v>211</v>
       </c>
       <c r="B50" s="7">
         <v>44316</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>25</v>
@@ -7282,19 +7282,19 @@
     </row>
     <row r="51" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>103</v>
+        <v>212</v>
       </c>
       <c r="B51" s="7">
         <v>44316</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>25</v>
@@ -7312,19 +7312,19 @@
     </row>
     <row r="52" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>104</v>
+        <v>213</v>
       </c>
       <c r="B52" s="7">
         <v>44316</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>25</v>
@@ -7342,19 +7342,19 @@
     </row>
     <row r="53" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>105</v>
+        <v>214</v>
       </c>
       <c r="B53" s="7">
         <v>44316</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>25</v>
@@ -7372,19 +7372,19 @@
     </row>
     <row r="54" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>106</v>
+        <v>215</v>
       </c>
       <c r="B54" s="7">
         <v>44316</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>25</v>
@@ -7402,19 +7402,19 @@
     </row>
     <row r="55" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="B55" s="7">
         <v>44316</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>25</v>
@@ -7432,19 +7432,19 @@
     </row>
     <row r="56" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>108</v>
+        <v>217</v>
       </c>
       <c r="B56" s="7">
         <v>44316</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>25</v>
@@ -7462,19 +7462,19 @@
     </row>
     <row r="57" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="B57" s="7">
         <v>44316</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>25</v>
@@ -7492,19 +7492,19 @@
     </row>
     <row r="58" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="B58" s="7">
         <v>44316</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>25</v>
@@ -7522,19 +7522,19 @@
     </row>
     <row r="59" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>111</v>
+        <v>220</v>
       </c>
       <c r="B59" s="7">
         <v>44316</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>25</v>
@@ -7552,19 +7552,19 @@
     </row>
     <row r="60" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="B60" s="7">
         <v>44316</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>25</v>
@@ -7582,19 +7582,19 @@
     </row>
     <row r="61" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="B61" s="7">
         <v>44316</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>25</v>
@@ -7612,19 +7612,19 @@
     </row>
     <row r="62" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B62" s="10">
         <v>44154</v>
       </c>
       <c r="C62" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>26</v>
@@ -7656,19 +7656,19 @@
     </row>
     <row r="63" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="9" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B63" s="10">
         <v>44154</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>26</v>
@@ -7700,19 +7700,19 @@
     </row>
     <row r="64" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B64" s="10">
         <v>44154</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>26</v>
@@ -7744,19 +7744,19 @@
     </row>
     <row r="65" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="9" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B65" s="10">
         <v>44154</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>26</v>
@@ -7788,19 +7788,19 @@
     </row>
     <row r="66" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="9" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B66" s="10">
         <v>44154</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>26</v>
@@ -7832,19 +7832,19 @@
     </row>
     <row r="67" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="B67" s="10">
         <v>44154</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>26</v>
@@ -7876,19 +7876,19 @@
     </row>
     <row r="68" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B68" s="10">
         <v>44154</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>26</v>
@@ -7920,19 +7920,19 @@
     </row>
     <row r="69" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B69" s="10">
         <v>44154</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>26</v>
@@ -7964,19 +7964,19 @@
     </row>
     <row r="70" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="B70" s="10">
         <v>44154</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>26</v>
@@ -8008,19 +8008,19 @@
     </row>
     <row r="71" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B71" s="10">
         <v>44154</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>26</v>
@@ -8052,19 +8052,19 @@
     </row>
     <row r="72" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B72" s="10">
         <v>44154</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>26</v>
@@ -8096,19 +8096,19 @@
     </row>
     <row r="73" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="B73" s="10">
         <v>44154</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>26</v>
@@ -8140,19 +8140,19 @@
     </row>
     <row r="74" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B74" s="10">
         <v>44154</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>26</v>
@@ -8184,19 +8184,19 @@
     </row>
     <row r="75" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B75" s="10">
         <v>44154</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>26</v>
@@ -8228,19 +8228,19 @@
     </row>
     <row r="76" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="B76" s="10">
         <v>44154</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>26</v>
@@ -8272,19 +8272,19 @@
     </row>
     <row r="77" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="B77" s="10">
         <v>44154</v>
       </c>
       <c r="C77" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="E77" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>29</v>
@@ -8316,19 +8316,19 @@
     </row>
     <row r="78" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="B78" s="10">
         <v>44154</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>29</v>
@@ -8360,19 +8360,19 @@
     </row>
     <row r="79" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="9" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B79" s="10">
         <v>44154</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>29</v>
@@ -8404,19 +8404,19 @@
     </row>
     <row r="80" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="B80" s="10">
         <v>44154</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>29</v>
@@ -8448,19 +8448,19 @@
     </row>
     <row r="81" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="B81" s="10">
         <v>44154</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>29</v>
@@ -8492,19 +8492,19 @@
     </row>
     <row r="82" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="9" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B82" s="10">
         <v>44154</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>29</v>
@@ -8536,19 +8536,19 @@
     </row>
     <row r="83" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="9" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="B83" s="10">
         <v>44154</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>29</v>
@@ -8580,19 +8580,19 @@
     </row>
     <row r="84" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B84" s="10">
         <v>44154</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F84" s="9" t="s">
         <v>29</v>
@@ -8624,19 +8624,19 @@
     </row>
     <row r="85" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="B85" s="10">
         <v>44154</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F85" s="9" t="s">
         <v>29</v>
@@ -8668,19 +8668,19 @@
     </row>
     <row r="86" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="9" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="B86" s="10">
         <v>44154</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F86" s="9" t="s">
         <v>29</v>
@@ -8712,19 +8712,19 @@
     </row>
     <row r="87" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="9" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B87" s="10">
         <v>44154</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>29</v>
@@ -8756,19 +8756,19 @@
     </row>
     <row r="88" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="9" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B88" s="10">
         <v>44154</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>29</v>
@@ -8800,19 +8800,19 @@
     </row>
     <row r="89" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="9" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B89" s="10">
         <v>44154</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>29</v>
@@ -8844,19 +8844,19 @@
     </row>
     <row r="90" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A90" s="9" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B90" s="10">
         <v>44154</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>29</v>
@@ -8888,19 +8888,19 @@
     </row>
     <row r="91" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="9" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B91" s="10">
         <v>44154</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>29</v>
@@ -8932,19 +8932,19 @@
     </row>
     <row r="92" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="9" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="B92" s="10">
         <v>44169</v>
       </c>
       <c r="C92" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D92" s="9" t="s">
+      <c r="E92" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>30</v>
@@ -8976,19 +8976,19 @@
     </row>
     <row r="93" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="9" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="B93" s="10">
         <v>44169</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>30</v>
@@ -9020,19 +9020,19 @@
     </row>
     <row r="94" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="9" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
       <c r="B94" s="10">
         <v>44169</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>30</v>
@@ -9064,19 +9064,19 @@
     </row>
     <row r="95" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="9" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="B95" s="10">
         <v>44169</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>30</v>
@@ -9108,19 +9108,19 @@
     </row>
     <row r="96" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A96" s="9" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="B96" s="10">
         <v>44169</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>30</v>
@@ -9152,19 +9152,19 @@
     </row>
     <row r="97" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="9" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
       <c r="B97" s="10">
         <v>44169</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F97" s="9" t="s">
         <v>30</v>
@@ -9196,19 +9196,19 @@
     </row>
     <row r="98" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="9" t="s">
-        <v>199</v>
+        <v>109</v>
       </c>
       <c r="B98" s="10">
         <v>44169</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>30</v>
@@ -9240,19 +9240,19 @@
     </row>
     <row r="99" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A99" s="9" t="s">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="B99" s="10">
         <v>44169</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F99" s="9" t="s">
         <v>30</v>
@@ -9284,19 +9284,19 @@
     </row>
     <row r="100" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="9" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B100" s="10">
         <v>44169</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F100" s="9" t="s">
         <v>30</v>
@@ -9328,19 +9328,19 @@
     </row>
     <row r="101" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="9" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="B101" s="10">
         <v>44169</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>30</v>
@@ -9372,19 +9372,19 @@
     </row>
     <row r="102" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="9" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
       <c r="B102" s="10">
         <v>44169</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F102" s="9" t="s">
         <v>30</v>
@@ -9416,19 +9416,19 @@
     </row>
     <row r="103" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="9" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B103" s="10">
         <v>44169</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F103" s="9" t="s">
         <v>30</v>
@@ -9460,19 +9460,19 @@
     </row>
     <row r="104" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="9" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
       <c r="B104" s="10">
         <v>44169</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F104" s="9" t="s">
         <v>30</v>
@@ -9504,19 +9504,19 @@
     </row>
     <row r="105" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="9" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="B105" s="10">
         <v>44169</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>30</v>
@@ -9548,19 +9548,19 @@
     </row>
     <row r="106" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="9" t="s">
-        <v>207</v>
+        <v>117</v>
       </c>
       <c r="B106" s="10">
         <v>44169</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F106" s="9" t="s">
         <v>30</v>
@@ -9592,19 +9592,19 @@
     </row>
     <row r="107" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="9" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="B107" s="10">
         <v>44169</v>
       </c>
       <c r="C107" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="9" t="s">
+      <c r="E107" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F107" s="9" t="s">
         <v>31</v>
@@ -9636,19 +9636,19 @@
     </row>
     <row r="108" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="9" t="s">
-        <v>209</v>
+        <v>119</v>
       </c>
       <c r="B108" s="10">
         <v>44169</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F108" s="9" t="s">
         <v>31</v>
@@ -9680,19 +9680,19 @@
     </row>
     <row r="109" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="9" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
       <c r="B109" s="10">
         <v>44169</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F109" s="9" t="s">
         <v>31</v>
@@ -9724,19 +9724,19 @@
     </row>
     <row r="110" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A110" s="9" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
       <c r="B110" s="10">
         <v>44169</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>31</v>
@@ -9768,19 +9768,19 @@
     </row>
     <row r="111" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="9" t="s">
-        <v>212</v>
+        <v>122</v>
       </c>
       <c r="B111" s="10">
         <v>44169</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F111" s="9" t="s">
         <v>31</v>
@@ -9812,19 +9812,19 @@
     </row>
     <row r="112" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A112" s="9" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="B112" s="10">
         <v>44169</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" s="9" t="s">
         <v>31</v>
@@ -9856,19 +9856,19 @@
     </row>
     <row r="113" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="9" t="s">
-        <v>214</v>
+        <v>124</v>
       </c>
       <c r="B113" s="10">
         <v>44169</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" s="9" t="s">
         <v>31</v>
@@ -9900,19 +9900,19 @@
     </row>
     <row r="114" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A114" s="9" t="s">
-        <v>215</v>
+        <v>125</v>
       </c>
       <c r="B114" s="10">
         <v>44169</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F114" s="9" t="s">
         <v>31</v>
@@ -9944,19 +9944,19 @@
     </row>
     <row r="115" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="9" t="s">
-        <v>216</v>
+        <v>126</v>
       </c>
       <c r="B115" s="10">
         <v>44169</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F115" s="9" t="s">
         <v>31</v>
@@ -9988,19 +9988,19 @@
     </row>
     <row r="116" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="9" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="B116" s="10">
         <v>44169</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F116" s="9" t="s">
         <v>31</v>
@@ -10032,19 +10032,19 @@
     </row>
     <row r="117" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="9" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="B117" s="10">
         <v>44169</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F117" s="9" t="s">
         <v>31</v>
@@ -10076,19 +10076,19 @@
     </row>
     <row r="118" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A118" s="9" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="B118" s="10">
         <v>44169</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F118" s="9" t="s">
         <v>31</v>
@@ -10120,19 +10120,19 @@
     </row>
     <row r="119" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="9" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="B119" s="10">
         <v>44169</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F119" s="9" t="s">
         <v>31</v>
@@ -10164,19 +10164,19 @@
     </row>
     <row r="120" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A120" s="9" t="s">
-        <v>221</v>
+        <v>131</v>
       </c>
       <c r="B120" s="10">
         <v>44169</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F120" s="9" t="s">
         <v>31</v>
@@ -10208,19 +10208,19 @@
     </row>
     <row r="121" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A121" s="9" t="s">
-        <v>222</v>
+        <v>132</v>
       </c>
       <c r="B121" s="10">
         <v>44169</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F121" s="9" t="s">
         <v>31</v>
@@ -15333,7 +15333,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -15365,7 +15365,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -15393,10 +15393,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="5"/>
@@ -15424,295 +15424,295 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>153</v>
+        <v>63</v>
       </c>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>157</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
-        <v>159</v>
+        <v>69</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>160</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="16" t="s">
-        <v>161</v>
+        <v>71</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>162</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>165</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>166</v>
+        <v>76</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>167</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>168</v>
+        <v>78</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>172</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>173</v>
+        <v>83</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>178</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>182</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>183</v>
+        <v>93</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>184</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>